<commit_message>
Added GetLastNonEmptyRowIndex and GetNonEmptyRowsForWorksheetfunctions
</commit_message>
<xml_diff>
--- a/C#/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
+++ b/C#/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\e-ASTC\Jlg.Common\JlgCommonTests\ExcelManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\jlg-common\C#\JlgCommonTests\ExcelManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="1" r:id="rId1"/>
     <sheet name="Page2" sheetId="2" r:id="rId2"/>
     <sheet name="Page3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t/>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>searchedString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -619,10 +624,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -653,6 +658,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C2"/>

</xml_diff>

<commit_message>
AGetColumnIndexesContainingStringValueded functions to get the coordinates of a string value (row and column) and to get the entire worksheet content and a method to add a list of cells
</commit_message>
<xml_diff>
--- a/C#/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
+++ b/C#/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="1" r:id="rId1"/>
     <sheet name="Page2" sheetId="2" r:id="rId2"/>
     <sheet name="Page3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t/>
   </si>
@@ -57,13 +57,67 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>State:</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Reporting Year:</t>
+  </si>
+  <si>
+    <t>Date of completion:</t>
+  </si>
+  <si>
+    <t>30/06/2015</t>
+  </si>
+  <si>
+    <t>Contact Person:</t>
+  </si>
+  <si>
+    <t>Dr. Martina Sahliger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position/Title </t>
+  </si>
+  <si>
+    <t>Organisation:</t>
+  </si>
+  <si>
+    <t>Bundesaufsichtsamt für Flugsicherung</t>
+  </si>
+  <si>
+    <t>Address:</t>
+  </si>
+  <si>
+    <t>Robert-Bosch-Str. 28, 63225 Langen, GERMANY</t>
+  </si>
+  <si>
+    <t>Tel:</t>
+  </si>
+  <si>
+    <t>+4961038043232</t>
+  </si>
+  <si>
+    <t>Fax:</t>
+  </si>
+  <si>
+    <t>+496103804344232</t>
+  </si>
+  <si>
+    <t>E-mail:</t>
+  </si>
+  <si>
+    <t>Martina.Sahliger@baf.bund.de</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,8 +133,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,6 +149,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -197,6 +268,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,9 +564,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -517,7 +597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +614,7 @@
         <v>7.3244999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -545,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +633,7 @@
         <v>42101</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,50 +651,156 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="11">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -630,27 +816,27 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -658,7 +844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Updated NuGet Packages and implemented fixes corresponding to the new package interfaces
</commit_message>
<xml_diff>
--- a/C#/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
+++ b/C#/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="1" r:id="rId1"/>
     <sheet name="Page2" sheetId="2" r:id="rId2"/>
     <sheet name="Page3" sheetId="3" r:id="rId3"/>
+    <sheet name="Page4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t/>
   </si>
@@ -111,6 +112,48 @@
   </si>
   <si>
     <t>Martina.Sahliger@baf.bund.de</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>getting</t>
+  </si>
+  <si>
+    <t>worksheet</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of </t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -251,6 +294,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,15 +320,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -675,10 +718,10 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -686,17 +729,17 @@
       <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="5">
         <v>2015</v>
       </c>
     </row>
@@ -704,17 +747,17 @@
       <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -722,84 +765,84 @@
       <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -825,16 +868,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -855,4 +898,71 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>